<commit_message>
added new data on Sivitinjavtanmililib2
</commit_message>
<xml_diff>
--- a/raw/concept_mapping.xlsx
+++ b/raw/concept_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bibiko/Documents/Developments/DLCE/lexibank/vanuatuvoices/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4475BC-3C63-FC44-B089-32D4099B321B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876579B6-E86C-2E44-93C7-3084E37508B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="760" windowWidth="33920" windowHeight="21580" xr2:uid="{5A3C358A-0268-8E4B-8A6A-856DEB801F9E}"/>
   </bookViews>
@@ -884,7 +884,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2800" uniqueCount="2228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2800" uniqueCount="2227">
   <si>
     <t>org_gloss</t>
   </si>
@@ -6752,9 +6752,6 @@
   </si>
   <si>
     <t>_direction_sea</t>
-  </si>
-  <si>
-    <t>_traditonal_medecine</t>
   </si>
   <si>
     <t>_tsunami</t>
@@ -8007,8 +8004,8 @@
   <dimension ref="A1:E1127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A883" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B906" sqref="B906"/>
+      <pane ySplit="1" topLeftCell="A971" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B992" sqref="B992"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8132,7 +8129,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>2222</v>
+        <v>2221</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -8140,7 +8137,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>2222</v>
+        <v>2221</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -8148,7 +8145,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>2222</v>
+        <v>2221</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -8156,7 +8153,7 @@
         <v>21</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>2222</v>
+        <v>2221</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -8580,7 +8577,7 @@
         <v>93</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="C59" s="1">
         <v>1403</v>
@@ -8656,7 +8653,7 @@
         <v>109</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>2224</v>
+        <v>2223</v>
       </c>
       <c r="C64" s="1">
         <v>379</v>
@@ -8890,7 +8887,7 @@
         <v>148</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9045,7 +9042,7 @@
     </row>
     <row r="104" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
       <c r="B104" s="8" t="s">
         <v>1911</v>
@@ -9190,7 +9187,7 @@
     </row>
     <row r="118" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="B118" s="8" t="s">
         <v>1913</v>
@@ -9330,10 +9327,10 @@
     </row>
     <row r="134" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
-        <v>2201</v>
+        <v>2200</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9341,7 +9338,7 @@
         <v>216</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9349,7 +9346,7 @@
         <v>217</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9533,7 +9530,7 @@
         <v>254</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9541,7 +9538,7 @@
         <v>255</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9549,7 +9546,7 @@
         <v>256</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9562,7 +9559,7 @@
         <v>258</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9570,7 +9567,7 @@
         <v>259</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="C161" s="1">
         <v>1357</v>
@@ -9587,7 +9584,7 @@
         <v>262</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="C162" s="1">
         <v>1057</v>
@@ -9604,7 +9601,7 @@
         <v>265</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9612,7 +9609,7 @@
         <v>266</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9620,7 +9617,7 @@
         <v>267</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9628,7 +9625,7 @@
         <v>268</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9636,7 +9633,7 @@
         <v>269</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9644,7 +9641,7 @@
         <v>270</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9652,7 +9649,7 @@
         <v>271</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="C169" s="1">
         <v>2703</v>
@@ -9669,7 +9666,7 @@
         <v>272</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="C170" s="1">
         <v>2703</v>
@@ -9686,7 +9683,7 @@
         <v>273</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="C171" s="1">
         <v>2703</v>
@@ -9703,7 +9700,7 @@
         <v>1846</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="C172" s="1">
         <v>2703</v>
@@ -9720,7 +9717,7 @@
         <v>270</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9796,7 +9793,7 @@
         <v>280</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="C178" s="1">
         <v>1179</v>
@@ -9830,7 +9827,7 @@
         <v>284</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9838,7 +9835,7 @@
         <v>285</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9856,7 +9853,7 @@
         <v>288</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9864,7 +9861,7 @@
         <v>289</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9872,7 +9869,7 @@
         <v>291</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9880,15 +9877,15 @@
         <v>290</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9896,7 +9893,7 @@
         <v>292</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -9909,7 +9906,7 @@
         <v>294</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="C191" s="1">
         <v>676</v>
@@ -9926,7 +9923,7 @@
         <v>297</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="C192" s="1">
         <v>3917</v>
@@ -9981,7 +9978,7 @@
         <v>305</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="C197" s="1">
         <v>597</v>
@@ -9998,7 +9995,7 @@
         <v>308</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="C198" s="1">
         <v>1479</v>
@@ -10020,7 +10017,7 @@
         <v>312</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10028,7 +10025,7 @@
         <v>313</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="202" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10092,7 +10089,7 @@
         <v>321</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="C206" s="1">
         <v>452</v>
@@ -10109,7 +10106,7 @@
         <v>323</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="C207" s="1">
         <v>452</v>
@@ -10126,7 +10123,7 @@
         <v>322</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="C208" s="1">
         <v>452</v>
@@ -10143,7 +10140,7 @@
         <v>324</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="210" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10151,7 +10148,7 @@
         <v>325</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="211" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10195,10 +10192,10 @@
     </row>
     <row r="214" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="4" t="s">
-        <v>2196</v>
+        <v>2195</v>
       </c>
       <c r="B214" s="8" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="215" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10206,7 +10203,7 @@
         <v>335</v>
       </c>
       <c r="B215" s="8" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10214,7 +10211,7 @@
         <v>336</v>
       </c>
       <c r="B216" s="8" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="217" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10222,7 +10219,7 @@
         <v>337</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="218" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10230,7 +10227,7 @@
         <v>338</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="219" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10238,7 +10235,7 @@
         <v>339</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="C219" s="1">
         <v>6</v>
@@ -10255,7 +10252,7 @@
         <v>342</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="C220" s="1">
         <v>1877</v>
@@ -10272,7 +10269,7 @@
         <v>345</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="C221" s="1">
         <v>1013</v>
@@ -10289,7 +10286,7 @@
         <v>346</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="C222" s="1">
         <v>1013</v>
@@ -10323,7 +10320,7 @@
         <v>18</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="C224" s="1">
         <v>1713</v>
@@ -10340,7 +10337,7 @@
         <v>353</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="C225" s="1">
         <v>1713</v>
@@ -10357,7 +10354,7 @@
         <v>80</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="C226" s="1">
         <v>1722</v>
@@ -10374,7 +10371,7 @@
         <v>356</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="C227" s="1">
         <v>1722</v>
@@ -10401,7 +10398,7 @@
         <v>11</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="C230" s="1">
         <v>1706</v>
@@ -10418,7 +10415,7 @@
         <v>361</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="C231" s="1">
         <v>1706</v>
@@ -10482,7 +10479,7 @@
         <v>374</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="D236" s="6" t="s">
         <v>533</v>
@@ -10538,7 +10535,7 @@
         <v>381</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="241" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10571,7 +10568,7 @@
         <v>384</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="C243" s="1">
         <v>2173</v>
@@ -10588,7 +10585,7 @@
         <v>385</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="245" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10601,7 +10598,7 @@
         <v>387</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="247" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10609,7 +10606,7 @@
         <v>388</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="248" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10617,7 +10614,7 @@
         <v>389</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="249" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10625,7 +10622,7 @@
         <v>390</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="250" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10633,7 +10630,7 @@
         <v>391</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="251" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10641,7 +10638,7 @@
         <v>392</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="252" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10649,7 +10646,7 @@
         <v>393</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="253" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10657,7 +10654,7 @@
         <v>394</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="254" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10665,7 +10662,7 @@
         <v>395</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="255" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10673,7 +10670,7 @@
         <v>396</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="C255" s="1">
         <v>2173</v>
@@ -10698,7 +10695,7 @@
         <v>398</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10706,7 +10703,7 @@
         <v>399</v>
       </c>
       <c r="B258" s="9" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10714,7 +10711,7 @@
         <v>400</v>
       </c>
       <c r="B259" s="9" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10722,7 +10719,7 @@
         <v>401</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10730,7 +10727,7 @@
         <v>402</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10738,7 +10735,7 @@
         <v>403</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10746,7 +10743,7 @@
         <v>404</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10754,7 +10751,7 @@
         <v>405</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10762,7 +10759,7 @@
         <v>406</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10770,7 +10767,7 @@
         <v>407</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10778,7 +10775,7 @@
         <v>408</v>
       </c>
       <c r="B267" s="9" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10786,7 +10783,7 @@
         <v>409</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10794,7 +10791,7 @@
         <v>410</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10802,7 +10799,7 @@
         <v>411</v>
       </c>
       <c r="B270" s="9" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10810,7 +10807,7 @@
         <v>412</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10818,7 +10815,7 @@
         <v>413</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="273" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10826,7 +10823,7 @@
         <v>414</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="274" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10834,7 +10831,7 @@
         <v>415</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="275" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10842,7 +10839,7 @@
         <v>416</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="276" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10850,7 +10847,7 @@
         <v>417</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="277" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10858,7 +10855,7 @@
         <v>418</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="278" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10866,7 +10863,7 @@
         <v>419</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="279" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10874,7 +10871,7 @@
         <v>420</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="280" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10882,7 +10879,7 @@
         <v>421</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="281" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10890,7 +10887,7 @@
         <v>422</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="282" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10898,7 +10895,7 @@
         <v>423</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="283" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10914,7 +10911,7 @@
         <v>425</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C284" s="1">
         <v>2262</v>
@@ -10931,7 +10928,7 @@
         <v>15</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C285" s="1">
         <v>1709</v>
@@ -10948,7 +10945,7 @@
         <v>428</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C286" s="1">
         <v>1709</v>
@@ -10999,7 +10996,7 @@
         <v>435</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C289" s="1">
         <v>2902</v>
@@ -11121,7 +11118,7 @@
         <v>461</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C302" s="1">
         <v>2003</v>
@@ -11163,15 +11160,15 @@
         <v>469</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="306" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A306" s="4" t="s">
-        <v>2205</v>
+        <v>2204</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="307" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11179,7 +11176,7 @@
         <v>470</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="308" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11214,7 +11211,7 @@
         <v>14</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C311" s="1">
         <v>2451</v>
@@ -11231,7 +11228,7 @@
         <v>477</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C312" s="1">
         <v>2451</v>
@@ -11248,7 +11245,7 @@
         <v>40</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="314" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11256,7 +11253,7 @@
         <v>480</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="315" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11281,7 +11278,7 @@
         <v>485</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="317" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11289,7 +11286,7 @@
         <v>486</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="318" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11297,7 +11294,7 @@
         <v>487</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C318" s="1">
         <v>586</v>
@@ -11314,7 +11311,7 @@
         <v>490</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="320" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11355,7 +11352,7 @@
         <v>498</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="C323" s="1">
         <v>2982</v>
@@ -11387,7 +11384,7 @@
         <v>504</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="328" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11395,7 +11392,7 @@
         <v>505</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="C328" s="1">
         <v>3231</v>
@@ -11429,7 +11426,7 @@
         <v>512</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="331" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11437,7 +11434,7 @@
         <v>513</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="332" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11445,7 +11442,7 @@
         <v>514</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="C332" s="1">
         <v>1383</v>
@@ -11462,7 +11459,7 @@
         <v>517</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="334" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11470,7 +11467,7 @@
         <v>518</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="335" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11478,7 +11475,7 @@
         <v>519</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="336" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11486,7 +11483,7 @@
         <v>520</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="337" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11494,7 +11491,7 @@
         <v>521</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="338" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11502,7 +11499,7 @@
         <v>522</v>
       </c>
       <c r="B338" s="8" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="339" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11551,7 +11548,7 @@
         <v>532</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="C343" s="1">
         <v>1282</v>
@@ -11590,7 +11587,7 @@
         <v>540</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="347" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11598,7 +11595,7 @@
         <v>541</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="348" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11631,7 +11628,7 @@
         <v>546</v>
       </c>
       <c r="B350" s="10" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="C350" s="1">
         <v>479</v>
@@ -11682,7 +11679,7 @@
         <v>556</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="354" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11690,7 +11687,7 @@
         <v>557</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="355" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11758,7 +11755,7 @@
         <v>571</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C361" s="1">
         <v>1223</v>
@@ -11775,7 +11772,7 @@
         <v>572</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C362" s="1">
         <v>1223</v>
@@ -11903,7 +11900,7 @@
         <v>597</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="C375" s="1">
         <v>683</v>
@@ -11920,7 +11917,7 @@
         <v>600</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="377" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11958,7 +11955,7 @@
         <v>607</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="381" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11966,7 +11963,7 @@
         <v>608</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="382" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11974,7 +11971,7 @@
         <v>609</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="383" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11982,7 +11979,7 @@
         <v>610</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="384" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11990,7 +11987,7 @@
         <v>611</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="385" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -11998,7 +11995,7 @@
         <v>612</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="386" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12006,7 +12003,7 @@
         <v>613</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="387" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12014,7 +12011,7 @@
         <v>614</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="388" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12044,7 +12041,7 @@
         <v>619</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="C390" s="1">
         <v>1459</v>
@@ -12085,15 +12082,15 @@
         <v>627</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="395" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A395" s="4" t="s">
-        <v>2220</v>
+        <v>2219</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="396" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12101,7 +12098,7 @@
         <v>628</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="397" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12109,7 +12106,7 @@
         <v>629</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="398" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12154,7 +12151,7 @@
         <v>637</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="404" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12162,7 +12159,7 @@
         <v>638</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="405" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12180,7 +12177,7 @@
         <v>641</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>2189</v>
+        <v>2188</v>
       </c>
       <c r="C407" s="1">
         <v>2248</v>
@@ -12191,7 +12188,7 @@
         <v>642</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="409" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12277,7 +12274,7 @@
         <v>660</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="416" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12285,15 +12282,15 @@
         <v>661</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="417" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A417" s="4" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="418" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12301,15 +12298,15 @@
         <v>662</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="419" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A419" s="4" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="420" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12317,7 +12314,7 @@
         <v>663</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="421" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12325,7 +12322,7 @@
         <v>664</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="422" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12333,7 +12330,7 @@
         <v>665</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12341,7 +12338,7 @@
         <v>666</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="424" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12349,7 +12346,7 @@
         <v>667</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="425" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12357,7 +12354,7 @@
         <v>668</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="426" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12365,7 +12362,7 @@
         <v>669</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="427" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12373,15 +12370,15 @@
         <v>670</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A428" s="4" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="429" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12389,7 +12386,7 @@
         <v>671</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12397,7 +12394,7 @@
         <v>672</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="431" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12405,7 +12402,7 @@
         <v>673</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="432" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12413,7 +12410,7 @@
         <v>674</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="433" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12421,15 +12418,15 @@
         <v>675</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="434" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A434" s="4" t="s">
-        <v>2219</v>
+        <v>2218</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="435" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12437,7 +12434,7 @@
         <v>676</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="436" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12445,15 +12442,15 @@
         <v>677</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="437" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A437" s="4" t="s">
-        <v>2218</v>
+        <v>2217</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="438" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12461,7 +12458,7 @@
         <v>678</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="439" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12474,7 +12471,7 @@
         <v>680</v>
       </c>
       <c r="B440" s="9" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="441" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12482,7 +12479,7 @@
         <v>681</v>
       </c>
       <c r="B441" s="9" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="442" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12490,7 +12487,7 @@
         <v>682</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="443" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12498,7 +12495,7 @@
         <v>683</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="444" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12506,7 +12503,7 @@
         <v>684</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="445" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12514,7 +12511,7 @@
         <v>685</v>
       </c>
       <c r="B445" s="9" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="446" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12561,7 +12558,7 @@
         <v>695</v>
       </c>
       <c r="B449" s="1" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="450" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12569,7 +12566,7 @@
         <v>696</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="451" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12577,7 +12574,7 @@
         <v>697</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="452" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12610,7 +12607,7 @@
         <v>703</v>
       </c>
       <c r="B454" s="8" t="s">
-        <v>2149</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="455" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12618,7 +12615,7 @@
         <v>704</v>
       </c>
       <c r="B455" s="8" t="s">
-        <v>2149</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="456" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12684,7 +12681,7 @@
         <v>718</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="C461" s="1">
         <v>2397</v>
@@ -12701,7 +12698,7 @@
         <v>721</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="463" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12709,7 +12706,7 @@
         <v>722</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="C463" s="1">
         <v>1203</v>
@@ -12720,7 +12717,7 @@
         <v>723</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="465" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12728,7 +12725,7 @@
         <v>724</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="466" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12736,7 +12733,7 @@
         <v>725</v>
       </c>
       <c r="B466" s="1" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="467" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12744,7 +12741,7 @@
         <v>726</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="C467" s="1">
         <v>2640</v>
@@ -12813,7 +12810,7 @@
         <v>738</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="474" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12821,7 +12818,7 @@
         <v>739</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="475" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12829,7 +12826,7 @@
         <v>740</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="476" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12837,7 +12834,7 @@
         <v>741</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="477" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12845,7 +12842,7 @@
         <v>742</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="C477" s="1">
         <v>925</v>
@@ -12862,7 +12859,7 @@
         <v>745</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="C478" s="1">
         <v>925</v>
@@ -12879,7 +12876,7 @@
         <v>746</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="C479" s="1">
         <v>2005</v>
@@ -12896,7 +12893,7 @@
         <v>747</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="C480" s="1">
         <v>2005</v>
@@ -12913,7 +12910,7 @@
         <v>750</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="C481" s="1">
         <v>195</v>
@@ -12957,7 +12954,7 @@
         <v>758</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="C485" s="1">
         <v>2615</v>
@@ -12974,7 +12971,7 @@
         <v>761</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="487" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12982,15 +12979,15 @@
         <v>762</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="488" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A488" s="4" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="489" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -12998,7 +12995,7 @@
         <v>763</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="490" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13006,7 +13003,7 @@
         <v>764</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="491" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13014,7 +13011,7 @@
         <v>765</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="492" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13022,7 +13019,7 @@
         <v>766</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="493" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13030,7 +13027,7 @@
         <v>767</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="494" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13038,7 +13035,7 @@
         <v>768</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="495" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13046,7 +13043,7 @@
         <v>769</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="496" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13054,7 +13051,7 @@
         <v>770</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="497" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13062,7 +13059,7 @@
         <v>771</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="C497" s="1">
         <v>766</v>
@@ -13079,7 +13076,7 @@
         <v>774</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="499" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13087,7 +13084,7 @@
         <v>775</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="C499" s="1">
         <v>249</v>
@@ -13231,7 +13228,7 @@
         <v>800</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="512" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13239,7 +13236,7 @@
         <v>801</v>
       </c>
       <c r="B512" s="1" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="513" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13247,7 +13244,7 @@
         <v>802</v>
       </c>
       <c r="B513" s="9" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="514" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13255,7 +13252,7 @@
         <v>803</v>
       </c>
       <c r="B514" s="9" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="515" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13263,7 +13260,7 @@
         <v>804</v>
       </c>
       <c r="B515" s="9" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="516" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13276,7 +13273,7 @@
         <v>806</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="518" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13284,7 +13281,7 @@
         <v>807</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="519" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13292,7 +13289,7 @@
         <v>808</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="520" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13316,7 +13313,7 @@
         <v>811</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="523" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13324,7 +13321,7 @@
         <v>812</v>
       </c>
       <c r="B523" s="9" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="524" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13332,7 +13329,7 @@
         <v>813</v>
       </c>
       <c r="B524" s="9" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="525" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13340,7 +13337,7 @@
         <v>814</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="526" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13348,7 +13345,7 @@
         <v>815</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="527" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13356,7 +13353,7 @@
         <v>816</v>
       </c>
       <c r="B527" s="1" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="528" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13364,7 +13361,7 @@
         <v>817</v>
       </c>
       <c r="B528" s="1" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="529" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13372,7 +13369,7 @@
         <v>818</v>
       </c>
       <c r="B529" s="1" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="530" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13380,7 +13377,7 @@
         <v>819</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="531" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13388,7 +13385,7 @@
         <v>820</v>
       </c>
       <c r="B531" s="1" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="532" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13396,7 +13393,7 @@
         <v>821</v>
       </c>
       <c r="B532" s="1" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="533" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13404,7 +13401,7 @@
         <v>822</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="534" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13412,7 +13409,7 @@
         <v>823</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="535" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13420,7 +13417,7 @@
         <v>824</v>
       </c>
       <c r="B535" s="1" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="536" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13428,7 +13425,7 @@
         <v>825</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="537" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13436,7 +13433,7 @@
         <v>826</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="538" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13452,7 +13449,7 @@
         <v>828</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="540" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13460,7 +13457,7 @@
         <v>829</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="541" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13468,7 +13465,7 @@
         <v>830</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="542" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13508,7 +13505,7 @@
         <v>838</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="547" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13524,7 +13521,7 @@
         <v>840</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="549" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13549,7 +13546,7 @@
         <v>845</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="D550" s="7" t="s">
         <v>1823</v>
@@ -13560,7 +13557,7 @@
         <v>846</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="C551" s="1">
         <v>1267</v>
@@ -13577,7 +13574,7 @@
         <v>849</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="553" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13585,15 +13582,15 @@
         <v>850</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="554" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A554" s="4" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="555" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13606,7 +13603,7 @@
         <v>852</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="557" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13614,7 +13611,7 @@
         <v>853</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="558" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13622,7 +13619,7 @@
         <v>854</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="559" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13664,7 +13661,7 @@
         <v>863</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
       <c r="C561" s="1">
         <v>1382</v>
@@ -13714,7 +13711,7 @@
         <v>872</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="C565" s="1">
         <v>3691</v>
@@ -13731,7 +13728,7 @@
         <v>873</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="C566" s="1">
         <v>3691</v>
@@ -13756,7 +13753,7 @@
         <v>877</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="569" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13781,7 +13778,7 @@
         <v>882</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="571" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13806,7 +13803,7 @@
         <v>19</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="C572" s="1">
         <v>1714</v>
@@ -13823,7 +13820,7 @@
         <v>887</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="C573" s="1">
         <v>1714</v>
@@ -13840,7 +13837,7 @@
         <v>90</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="C574" s="1">
         <v>1724</v>
@@ -13857,7 +13854,7 @@
         <v>890</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="C575" s="1">
         <v>1724</v>
@@ -13874,7 +13871,7 @@
         <v>893</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="C576" s="1">
         <v>796</v>
@@ -13908,7 +13905,7 @@
         <v>899</v>
       </c>
       <c r="B578" s="1" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="C578" s="1">
         <v>1598</v>
@@ -13942,7 +13939,7 @@
         <v>906</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="581" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13950,7 +13947,7 @@
         <v>907</v>
       </c>
       <c r="B581" s="1" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="582" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13958,7 +13955,7 @@
         <v>908</v>
       </c>
       <c r="B582" s="1" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="583" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -13971,7 +13968,7 @@
         <v>910</v>
       </c>
       <c r="B584" s="1" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="C584" s="1">
         <v>2581</v>
@@ -13988,7 +13985,7 @@
         <v>913</v>
       </c>
       <c r="B585" s="1" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="C585" s="1">
         <v>2581</v>
@@ -14002,10 +13999,10 @@
     </row>
     <row r="586" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A586" s="4" t="s">
-        <v>2212</v>
+        <v>2211</v>
       </c>
       <c r="B586" s="1" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="587" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14013,7 +14010,7 @@
         <v>914</v>
       </c>
       <c r="B587" s="1" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="588" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14021,7 +14018,7 @@
         <v>915</v>
       </c>
       <c r="B588" s="1" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="589" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14046,7 +14043,7 @@
         <v>920</v>
       </c>
       <c r="B590" s="1" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="591" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14054,7 +14051,7 @@
         <v>921</v>
       </c>
       <c r="B591" s="1" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="592" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14062,7 +14059,7 @@
         <v>922</v>
       </c>
       <c r="B592" s="1" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="593" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14070,7 +14067,7 @@
         <v>923</v>
       </c>
       <c r="B593" s="1" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="594" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14078,7 +14075,7 @@
         <v>924</v>
       </c>
       <c r="B594" s="1" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="595" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14086,7 +14083,7 @@
         <v>925</v>
       </c>
       <c r="B595" s="1" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="596" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14094,7 +14091,7 @@
         <v>926</v>
       </c>
       <c r="B596" s="1" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="597" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14102,7 +14099,7 @@
         <v>927</v>
       </c>
       <c r="B597" s="1" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="598" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14131,7 +14128,7 @@
         <v>931</v>
       </c>
       <c r="B601" s="1" t="s">
-        <v>2103</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="602" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14139,7 +14136,7 @@
         <v>932</v>
       </c>
       <c r="B602" s="1" t="s">
-        <v>2104</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="603" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14147,7 +14144,7 @@
         <v>933</v>
       </c>
       <c r="B603" s="1" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="604" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14155,7 +14152,7 @@
         <v>934</v>
       </c>
       <c r="B604" s="1" t="s">
-        <v>2103</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="605" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14187,7 +14184,7 @@
         <v>938</v>
       </c>
       <c r="B608" s="1" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="609" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14195,7 +14192,7 @@
         <v>939</v>
       </c>
       <c r="B609" s="1" t="s">
-        <v>2103</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="610" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14213,7 +14210,7 @@
         <v>942</v>
       </c>
       <c r="B612" s="1" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="613" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14244,7 +14241,7 @@
         <v>947</v>
       </c>
       <c r="B617" s="1" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="618" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14252,7 +14249,7 @@
         <v>948</v>
       </c>
       <c r="B618" s="1" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="619" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14260,7 +14257,7 @@
         <v>949</v>
       </c>
       <c r="B619" s="1" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="620" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14268,7 +14265,7 @@
         <v>950</v>
       </c>
       <c r="B620" s="1" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="621" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14276,7 +14273,7 @@
         <v>951</v>
       </c>
       <c r="B621" s="1" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="622" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14294,7 +14291,7 @@
         <v>954</v>
       </c>
       <c r="B624" s="1" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="625" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14302,7 +14299,7 @@
         <v>955</v>
       </c>
       <c r="B625" s="1" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="626" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14310,7 +14307,7 @@
         <v>956</v>
       </c>
       <c r="B626" s="1" t="s">
-        <v>2109</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="627" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14328,7 +14325,7 @@
         <v>959</v>
       </c>
       <c r="B629" s="1" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="630" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14336,7 +14333,7 @@
         <v>960</v>
       </c>
       <c r="B630" s="1" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="631" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14344,7 +14341,7 @@
         <v>961</v>
       </c>
       <c r="B631" s="1" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="632" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14352,7 +14349,7 @@
         <v>962</v>
       </c>
       <c r="B632" s="1" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="633" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14360,7 +14357,7 @@
         <v>963</v>
       </c>
       <c r="B633" s="1" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="634" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14373,7 +14370,7 @@
         <v>965</v>
       </c>
       <c r="B635" s="1" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="636" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14389,7 +14386,7 @@
         <v>967</v>
       </c>
       <c r="B637" s="1" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="638" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14397,7 +14394,7 @@
         <v>968</v>
       </c>
       <c r="B638" s="1" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="639" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14523,7 +14520,7 @@
         <v>987</v>
       </c>
       <c r="B647" s="1" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="C647" s="1">
         <v>416</v>
@@ -14540,7 +14537,7 @@
         <v>990</v>
       </c>
       <c r="B648" s="1" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="C648" s="1">
         <v>1143</v>
@@ -14557,7 +14554,7 @@
         <v>993</v>
       </c>
       <c r="B649" s="1" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="C649" s="1">
         <v>735</v>
@@ -14574,7 +14571,7 @@
         <v>994</v>
       </c>
       <c r="B650" s="1" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="C650" s="1">
         <v>735</v>
@@ -14591,7 +14588,7 @@
         <v>997</v>
       </c>
       <c r="B651" s="1" t="s">
-        <v>2116</v>
+        <v>2115</v>
       </c>
       <c r="C651" s="1">
         <v>3137</v>
@@ -14608,7 +14605,7 @@
         <v>1000</v>
       </c>
       <c r="B652" s="1" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="C652" s="1">
         <v>2561</v>
@@ -14625,7 +14622,7 @@
         <v>1003</v>
       </c>
       <c r="B653" s="1" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="654" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14638,7 +14635,7 @@
         <v>1005</v>
       </c>
       <c r="B655" s="1" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="656" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14659,7 +14656,7 @@
         <v>1008</v>
       </c>
       <c r="B658" s="1" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="C658" s="1">
         <v>1338</v>
@@ -14676,15 +14673,15 @@
         <v>1011</v>
       </c>
       <c r="B659" s="1" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="660" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A660" s="4" t="s">
-        <v>2209</v>
+        <v>2208</v>
       </c>
       <c r="B660" s="1" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="661" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14692,7 +14689,7 @@
         <v>1012</v>
       </c>
       <c r="B661" s="1" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="662" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14700,15 +14697,15 @@
         <v>1013</v>
       </c>
       <c r="B662" s="1" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="663" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A663" s="4" t="s">
-        <v>2215</v>
+        <v>2214</v>
       </c>
       <c r="B663" s="1" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="664" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14716,7 +14713,7 @@
         <v>1014</v>
       </c>
       <c r="B664" s="1" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="665" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14734,7 +14731,7 @@
         <v>1017</v>
       </c>
       <c r="B667" s="1" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
       <c r="C667" s="1">
         <v>1337</v>
@@ -14751,7 +14748,7 @@
         <v>1020</v>
       </c>
       <c r="B668" s="1" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
       <c r="C668" s="1">
         <v>1337</v>
@@ -14768,7 +14765,7 @@
         <v>1021</v>
       </c>
       <c r="B669" s="1" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
       <c r="C669" s="1">
         <v>1337</v>
@@ -14785,7 +14782,7 @@
         <v>1022</v>
       </c>
       <c r="B670" s="1" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="671" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14798,7 +14795,7 @@
         <v>1024</v>
       </c>
       <c r="B672" s="1" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
       <c r="C672" s="1">
         <v>2488</v>
@@ -14812,10 +14809,10 @@
     </row>
     <row r="673" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A673" s="4" t="s">
-        <v>2203</v>
+        <v>2202</v>
       </c>
       <c r="B673" s="1" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
       <c r="C673" s="1">
         <v>2488</v>
@@ -14832,7 +14829,7 @@
         <v>1025</v>
       </c>
       <c r="B674" s="1" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
       <c r="C674" s="1">
         <v>2488</v>
@@ -14849,7 +14846,7 @@
         <v>1028</v>
       </c>
       <c r="B675" s="1" t="s">
-        <v>2125</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="676" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14857,7 +14854,7 @@
         <v>1029</v>
       </c>
       <c r="B676" s="1" t="s">
-        <v>2125</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="677" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14865,15 +14862,15 @@
         <v>1030</v>
       </c>
       <c r="B677" s="1" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="678" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A678" s="4" t="s">
-        <v>2210</v>
+        <v>2209</v>
       </c>
       <c r="B678" s="1" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="679" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14881,7 +14878,7 @@
         <v>1031</v>
       </c>
       <c r="B679" s="1" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="680" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14889,7 +14886,7 @@
         <v>1032</v>
       </c>
       <c r="B680" s="1" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
       <c r="C680" s="1">
         <v>2487</v>
@@ -14903,10 +14900,10 @@
     </row>
     <row r="681" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A681" s="4" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="B681" s="1" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
       <c r="C681" s="1">
         <v>2487</v>
@@ -14923,7 +14920,7 @@
         <v>1033</v>
       </c>
       <c r="B682" s="1" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
       <c r="C682" s="1">
         <v>2487</v>
@@ -14950,7 +14947,7 @@
         <v>1038</v>
       </c>
       <c r="B685" s="1" t="s">
-        <v>2128</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="686" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14958,7 +14955,7 @@
         <v>1039</v>
       </c>
       <c r="B686" s="1" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="687" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -14987,7 +14984,7 @@
         <v>1043</v>
       </c>
       <c r="B690" s="1" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="C690" s="1">
         <v>3388</v>
@@ -15004,7 +15001,7 @@
         <v>1044</v>
       </c>
       <c r="B691" s="1" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="C691" s="1">
         <v>3388</v>
@@ -15021,7 +15018,7 @@
         <v>1047</v>
       </c>
       <c r="B692" s="1" t="s">
-        <v>2130</v>
+        <v>2129</v>
       </c>
       <c r="C692" s="1">
         <v>655</v>
@@ -15038,7 +15035,7 @@
         <v>1050</v>
       </c>
       <c r="B693" s="1" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="694" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15046,7 +15043,7 @@
         <v>1051</v>
       </c>
       <c r="B694" s="1" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="695" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15054,7 +15051,7 @@
         <v>1052</v>
       </c>
       <c r="B695" s="1" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="696" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15062,7 +15059,7 @@
         <v>1053</v>
       </c>
       <c r="B696" s="1" t="s">
-        <v>2132</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="697" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15070,7 +15067,7 @@
         <v>1054</v>
       </c>
       <c r="B697" s="1" t="s">
-        <v>2132</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="698" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15078,7 +15075,7 @@
         <v>1055</v>
       </c>
       <c r="B698" s="1" t="s">
-        <v>2133</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="699" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15110,7 +15107,7 @@
         <v>1061</v>
       </c>
       <c r="B702" s="1" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="C702" s="1">
         <v>3827</v>
@@ -15132,7 +15129,7 @@
         <v>1065</v>
       </c>
       <c r="B704" s="1" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="705" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15140,7 +15137,7 @@
         <v>1066</v>
       </c>
       <c r="B705" s="1" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="706" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15148,7 +15145,7 @@
         <v>1067</v>
       </c>
       <c r="B706" s="1" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="707" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15161,7 +15158,7 @@
         <v>1069</v>
       </c>
       <c r="B708" s="1" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="709" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15169,7 +15166,7 @@
         <v>1070</v>
       </c>
       <c r="B709" s="1" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="710" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15204,7 +15201,7 @@
         <v>1077</v>
       </c>
       <c r="B713" s="1" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="C713" s="1">
         <v>1733</v>
@@ -15268,7 +15265,7 @@
         <v>1090</v>
       </c>
       <c r="B718" s="1" t="s">
-        <v>2154</v>
+        <v>2153</v>
       </c>
       <c r="C718" s="1">
         <v>660</v>
@@ -15309,7 +15306,7 @@
         <v>1098</v>
       </c>
       <c r="B722" s="1" t="s">
-        <v>2155</v>
+        <v>2154</v>
       </c>
     </row>
     <row r="723" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15317,7 +15314,7 @@
         <v>1849</v>
       </c>
       <c r="B723" s="1" t="s">
-        <v>2155</v>
+        <v>2154</v>
       </c>
     </row>
     <row r="724" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15325,7 +15322,7 @@
         <v>1099</v>
       </c>
       <c r="B724" s="1" t="s">
-        <v>2155</v>
+        <v>2154</v>
       </c>
     </row>
     <row r="725" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15333,7 +15330,7 @@
         <v>1100</v>
       </c>
       <c r="B725" s="1" t="s">
-        <v>2155</v>
+        <v>2154</v>
       </c>
     </row>
     <row r="726" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15341,7 +15338,7 @@
         <v>1101</v>
       </c>
       <c r="B726" s="1" t="s">
-        <v>2190</v>
+        <v>2189</v>
       </c>
     </row>
     <row r="727" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15385,7 +15382,7 @@
         <v>1110</v>
       </c>
       <c r="B730" s="1" t="s">
-        <v>2156</v>
+        <v>2155</v>
       </c>
     </row>
     <row r="731" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15393,7 +15390,7 @@
         <v>1111</v>
       </c>
       <c r="B731" s="1" t="s">
-        <v>2157</v>
+        <v>2156</v>
       </c>
       <c r="C731" s="1">
         <v>2457</v>
@@ -15415,7 +15412,7 @@
         <v>1115</v>
       </c>
       <c r="B733" s="1" t="s">
-        <v>2158</v>
+        <v>2157</v>
       </c>
       <c r="C733" s="1">
         <v>670</v>
@@ -15476,7 +15473,7 @@
         <v>1128</v>
       </c>
       <c r="B738" s="1" t="s">
-        <v>2159</v>
+        <v>2158</v>
       </c>
       <c r="C738" s="1">
         <v>787</v>
@@ -15493,7 +15490,7 @@
         <v>1131</v>
       </c>
       <c r="B739" s="1" t="s">
-        <v>2160</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="740" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15501,7 +15498,7 @@
         <v>1132</v>
       </c>
       <c r="B740" s="1" t="s">
-        <v>2160</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="741" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15509,7 +15506,7 @@
         <v>1133</v>
       </c>
       <c r="B741" s="1" t="s">
-        <v>2161</v>
+        <v>2160</v>
       </c>
       <c r="C741" s="1">
         <v>1274</v>
@@ -15526,7 +15523,7 @@
         <v>1136</v>
       </c>
       <c r="B742" s="1" t="s">
-        <v>2162</v>
+        <v>2161</v>
       </c>
     </row>
     <row r="743" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15587,7 +15584,7 @@
         <v>1149</v>
       </c>
       <c r="B747" s="1" t="s">
-        <v>2161</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="748" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15595,15 +15592,15 @@
         <v>1150</v>
       </c>
       <c r="B748" s="1" t="s">
-        <v>2163</v>
+        <v>2162</v>
       </c>
     </row>
     <row r="749" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A749" s="4" t="s">
-        <v>2204</v>
+        <v>2203</v>
       </c>
       <c r="B749" s="1" t="s">
-        <v>2163</v>
+        <v>2162</v>
       </c>
     </row>
     <row r="750" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15611,7 +15608,7 @@
         <v>1151</v>
       </c>
       <c r="B750" s="1" t="s">
-        <v>2163</v>
+        <v>2162</v>
       </c>
     </row>
     <row r="751" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15619,7 +15616,7 @@
         <v>1152</v>
       </c>
       <c r="B751" s="1" t="s">
-        <v>2164</v>
+        <v>2163</v>
       </c>
       <c r="C751" s="1">
         <v>1121</v>
@@ -15636,7 +15633,7 @@
         <v>1153</v>
       </c>
       <c r="B752" s="1" t="s">
-        <v>2164</v>
+        <v>2163</v>
       </c>
       <c r="C752" s="1">
         <v>1121</v>
@@ -15687,7 +15684,7 @@
         <v>17</v>
       </c>
       <c r="B755" s="1" t="s">
-        <v>2165</v>
+        <v>2164</v>
       </c>
       <c r="C755" s="1">
         <v>2453</v>
@@ -15704,7 +15701,7 @@
         <v>1164</v>
       </c>
       <c r="B756" s="1" t="s">
-        <v>2165</v>
+        <v>2164</v>
       </c>
       <c r="C756" s="1">
         <v>2453</v>
@@ -15721,7 +15718,7 @@
         <v>70</v>
       </c>
       <c r="B757" s="1" t="s">
-        <v>2166</v>
+        <v>2165</v>
       </c>
       <c r="C757" s="1">
         <v>1721</v>
@@ -15738,7 +15735,7 @@
         <v>1167</v>
       </c>
       <c r="B758" s="1" t="s">
-        <v>2166</v>
+        <v>2165</v>
       </c>
       <c r="C758" s="1">
         <v>1721</v>
@@ -15755,7 +15752,7 @@
         <v>1170</v>
       </c>
       <c r="B759" s="1" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
     </row>
     <row r="760" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15794,7 +15791,7 @@
         <v>1177</v>
       </c>
       <c r="B762" s="1" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="C762" s="1">
         <v>1110</v>
@@ -15842,7 +15839,7 @@
         <v>1187</v>
       </c>
       <c r="B765" s="1" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
     </row>
     <row r="766" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15867,7 +15864,7 @@
         <v>1192</v>
       </c>
       <c r="B767" s="1" t="s">
-        <v>2169</v>
+        <v>2168</v>
       </c>
       <c r="C767" s="1">
         <v>1645</v>
@@ -15930,15 +15927,15 @@
         <v>1205</v>
       </c>
       <c r="B773" s="1" t="s">
-        <v>2170</v>
+        <v>2169</v>
       </c>
     </row>
     <row r="774" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A774" s="4" t="s">
-        <v>2213</v>
+        <v>2212</v>
       </c>
       <c r="B774" s="1" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="775" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15946,7 +15943,7 @@
         <v>1206</v>
       </c>
       <c r="B775" s="1" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="776" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15954,7 +15951,7 @@
         <v>1207</v>
       </c>
       <c r="B776" s="1" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="777" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15962,7 +15959,7 @@
         <v>1208</v>
       </c>
       <c r="B777" s="1" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="778" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15970,7 +15967,7 @@
         <v>1209</v>
       </c>
       <c r="B778" s="1" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="779" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15978,7 +15975,7 @@
         <v>1210</v>
       </c>
       <c r="B779" s="1" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="780" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -15986,7 +15983,7 @@
         <v>1211</v>
       </c>
       <c r="B780" s="1" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="781" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16010,7 +16007,7 @@
         <v>1214</v>
       </c>
       <c r="B783" s="1" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="784" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16034,7 +16031,7 @@
         <v>1217</v>
       </c>
       <c r="B786" s="1" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="C786" s="1">
         <v>1649</v>
@@ -16078,7 +16075,7 @@
         <v>16</v>
       </c>
       <c r="B790" s="1" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
       <c r="C790" s="1">
         <v>2454</v>
@@ -16095,7 +16092,7 @@
         <v>1226</v>
       </c>
       <c r="B791" s="1" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
       <c r="C791" s="1">
         <v>2454</v>
@@ -16112,7 +16109,7 @@
         <v>60</v>
       </c>
       <c r="B792" s="1" t="s">
-        <v>2174</v>
+        <v>2173</v>
       </c>
       <c r="C792" s="1">
         <v>1718</v>
@@ -16129,7 +16126,7 @@
         <v>1229</v>
       </c>
       <c r="B793" s="1" t="s">
-        <v>2174</v>
+        <v>2173</v>
       </c>
       <c r="C793" s="1">
         <v>1718</v>
@@ -16163,7 +16160,7 @@
         <v>1236</v>
       </c>
       <c r="B795" s="1" t="s">
-        <v>2175</v>
+        <v>2174</v>
       </c>
       <c r="C795" s="1">
         <v>1605</v>
@@ -16205,7 +16202,7 @@
         <v>1244</v>
       </c>
       <c r="B798" s="1" t="s">
-        <v>2176</v>
+        <v>2175</v>
       </c>
       <c r="C798" s="1">
         <v>812</v>
@@ -16309,7 +16306,7 @@
         <v>1267</v>
       </c>
       <c r="B805" s="1" t="s">
-        <v>2177</v>
+        <v>2176</v>
       </c>
       <c r="C805" s="1">
         <v>375</v>
@@ -16326,7 +16323,7 @@
         <v>1270</v>
       </c>
       <c r="B806" s="1" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
       <c r="C806" s="1">
         <v>1620</v>
@@ -16348,7 +16345,7 @@
         <v>1274</v>
       </c>
       <c r="B808" s="1" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="C808" s="1">
         <v>1056</v>
@@ -16365,7 +16362,7 @@
         <v>1277</v>
       </c>
       <c r="B809" s="1" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="810" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16373,7 +16370,7 @@
         <v>1278</v>
       </c>
       <c r="B810" s="1" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="811" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16381,7 +16378,7 @@
         <v>1850</v>
       </c>
       <c r="B811" s="1" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="812" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16389,7 +16386,7 @@
         <v>1279</v>
       </c>
       <c r="B812" s="1" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="813" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16397,7 +16394,7 @@
         <v>1280</v>
       </c>
       <c r="B813" s="1" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="814" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16405,7 +16402,7 @@
         <v>1281</v>
       </c>
       <c r="B814" s="1" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="815" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16413,7 +16410,7 @@
         <v>1282</v>
       </c>
       <c r="B815" s="1" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="816" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16421,7 +16418,7 @@
         <v>1283</v>
       </c>
       <c r="B816" s="1" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
     </row>
     <row r="817" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16429,7 +16426,7 @@
         <v>1284</v>
       </c>
       <c r="B817" s="1" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
     </row>
     <row r="818" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16437,7 +16434,7 @@
         <v>1285</v>
       </c>
       <c r="B818" s="1" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="819" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16445,7 +16442,7 @@
         <v>1286</v>
       </c>
       <c r="B819" s="1" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
     </row>
     <row r="820" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16453,7 +16450,7 @@
         <v>1287</v>
       </c>
       <c r="B820" s="1" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="821" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16461,7 +16458,7 @@
         <v>1288</v>
       </c>
       <c r="B821" s="1" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="822" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16493,7 +16490,7 @@
         <v>1294</v>
       </c>
       <c r="B825" s="1" t="s">
-        <v>2181</v>
+        <v>2180</v>
       </c>
       <c r="C825" s="1">
         <v>1595</v>
@@ -16510,7 +16507,7 @@
         <v>1297</v>
       </c>
       <c r="B826" s="1" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
       <c r="C826" s="1">
         <v>1351</v>
@@ -16527,7 +16524,7 @@
         <v>1300</v>
       </c>
       <c r="B827" s="1" t="s">
-        <v>2223</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="828" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16535,7 +16532,7 @@
         <v>1301</v>
       </c>
       <c r="B828" s="1" t="s">
-        <v>2223</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="829" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16560,7 +16557,7 @@
         <v>1306</v>
       </c>
       <c r="B830" s="1" t="s">
-        <v>2182</v>
+        <v>2181</v>
       </c>
     </row>
     <row r="831" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16568,7 +16565,7 @@
         <v>1307</v>
       </c>
       <c r="B831" s="1" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="832" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16576,7 +16573,7 @@
         <v>1308</v>
       </c>
       <c r="B832" s="1" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="833" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16584,7 +16581,7 @@
         <v>1309</v>
       </c>
       <c r="B833" s="1" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="834" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16592,7 +16589,7 @@
         <v>1310</v>
       </c>
       <c r="B834" s="1" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="835" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16600,7 +16597,7 @@
         <v>1311</v>
       </c>
       <c r="B835" s="1" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="836" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16608,7 +16605,7 @@
         <v>1312</v>
       </c>
       <c r="B836" s="1" t="s">
-        <v>2183</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="837" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16616,7 +16613,7 @@
         <v>1314</v>
       </c>
       <c r="B837" s="1" t="s">
-        <v>2183</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="838" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16624,7 +16621,7 @@
         <v>1313</v>
       </c>
       <c r="B838" s="1" t="s">
-        <v>2183</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="839" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16632,7 +16629,7 @@
         <v>1315</v>
       </c>
       <c r="B839" s="9" t="s">
-        <v>2184</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="840" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16694,7 +16691,7 @@
         <v>1328</v>
       </c>
       <c r="B846" s="1" t="s">
-        <v>2185</v>
+        <v>2184</v>
       </c>
       <c r="C846" s="1">
         <v>1251</v>
@@ -16743,7 +16740,7 @@
         <v>1338</v>
       </c>
       <c r="B851" s="1" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="852" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16751,7 +16748,7 @@
         <v>1339</v>
       </c>
       <c r="B852" s="1" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="853" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16759,7 +16756,7 @@
         <v>1340</v>
       </c>
       <c r="B853" s="1" t="s">
-        <v>2153</v>
+        <v>2152</v>
       </c>
       <c r="C853" s="1">
         <v>858</v>
@@ -16776,7 +16773,7 @@
         <v>1341</v>
       </c>
       <c r="B854" s="1" t="s">
-        <v>2153</v>
+        <v>2152</v>
       </c>
       <c r="C854" s="1">
         <v>858</v>
@@ -16793,7 +16790,7 @@
         <v>1344</v>
       </c>
       <c r="B855" s="1" t="s">
-        <v>2187</v>
+        <v>2186</v>
       </c>
       <c r="C855" s="1">
         <v>1404</v>
@@ -16815,7 +16812,7 @@
         <v>1348</v>
       </c>
       <c r="B857" s="1" t="s">
-        <v>2152</v>
+        <v>2151</v>
       </c>
       <c r="C857" s="1">
         <v>1421</v>
@@ -16832,7 +16829,7 @@
         <v>1351</v>
       </c>
       <c r="B858" s="1" t="s">
-        <v>2151</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="859" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16845,7 +16842,7 @@
         <v>1353</v>
       </c>
       <c r="B860" s="1" t="s">
-        <v>2150</v>
+        <v>2149</v>
       </c>
       <c r="C860" s="1">
         <v>1343</v>
@@ -16862,7 +16859,7 @@
         <v>1354</v>
       </c>
       <c r="B861" s="1" t="s">
-        <v>2150</v>
+        <v>2149</v>
       </c>
       <c r="C861" s="1">
         <v>1343</v>
@@ -16879,7 +16876,7 @@
         <v>1357</v>
       </c>
       <c r="B862" s="1" t="s">
-        <v>2149</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="863" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16892,7 +16889,7 @@
         <v>1359</v>
       </c>
       <c r="B864" s="1" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="865" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16944,7 +16941,7 @@
         <v>1370</v>
       </c>
       <c r="B869" s="1" t="s">
-        <v>2148</v>
+        <v>2147</v>
       </c>
       <c r="C869" s="1">
         <v>1265</v>
@@ -16966,7 +16963,7 @@
         <v>1374</v>
       </c>
       <c r="B871" s="1" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
     </row>
     <row r="872" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16974,7 +16971,7 @@
         <v>1375</v>
       </c>
       <c r="B872" s="1" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
     </row>
     <row r="873" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16982,7 +16979,7 @@
         <v>1376</v>
       </c>
       <c r="B873" s="1" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
     </row>
     <row r="874" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -16990,7 +16987,7 @@
         <v>1377</v>
       </c>
       <c r="B874" s="1" t="s">
-        <v>2145</v>
+        <v>2144</v>
       </c>
       <c r="C874" s="1">
         <v>68</v>
@@ -17049,7 +17046,7 @@
         <v>1389</v>
       </c>
       <c r="B878" s="1" t="s">
-        <v>2144</v>
+        <v>2143</v>
       </c>
       <c r="C878" s="1">
         <v>279</v>
@@ -17066,7 +17063,7 @@
         <v>1392</v>
       </c>
       <c r="B879" s="1" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
       <c r="C879" s="1">
         <v>817</v>
@@ -17083,7 +17080,7 @@
         <v>1395</v>
       </c>
       <c r="B880" s="1" t="s">
-        <v>2226</v>
+        <v>2225</v>
       </c>
     </row>
     <row r="881" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -17091,7 +17088,7 @@
         <v>1396</v>
       </c>
       <c r="B881" s="1" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="882" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -17099,7 +17096,7 @@
         <v>1397</v>
       </c>
       <c r="B882" s="1" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
     </row>
     <row r="883" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -17107,7 +17104,7 @@
         <v>1398</v>
       </c>
       <c r="B883" s="1" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="884" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -17115,7 +17112,7 @@
         <v>1399</v>
       </c>
       <c r="B884" s="10" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="C884" s="1">
         <v>2271</v>
@@ -17129,7 +17126,7 @@
         <v>13</v>
       </c>
       <c r="B885" s="1" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
       <c r="C885" s="1">
         <v>1708</v>
@@ -17146,7 +17143,7 @@
         <v>1400</v>
       </c>
       <c r="B886" s="1" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
       <c r="C886" s="1">
         <v>1708</v>
@@ -17163,7 +17160,7 @@
         <v>30</v>
       </c>
       <c r="B887" s="1" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="C887" s="1">
         <v>1715</v>
@@ -17180,7 +17177,7 @@
         <v>1403</v>
       </c>
       <c r="B888" s="1" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="C888" s="1">
         <v>1715</v>
@@ -17267,7 +17264,7 @@
         <v>1422</v>
       </c>
       <c r="B894" s="1" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="895" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -17277,7 +17274,7 @@
     </row>
     <row r="896" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A896" s="4" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="B896" s="1" t="s">
         <v>1940</v>
@@ -17304,7 +17301,7 @@
         <v>1426</v>
       </c>
       <c r="B899" s="1" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="900" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -17312,7 +17309,7 @@
         <v>1427</v>
       </c>
       <c r="B900" s="1" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="901" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -17320,7 +17317,7 @@
         <v>1428</v>
       </c>
       <c r="B901" s="1" t="s">
-        <v>2227</v>
+        <v>2226</v>
       </c>
     </row>
     <row r="902" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -17328,7 +17325,7 @@
         <v>1429</v>
       </c>
       <c r="B902" s="10" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="C902" s="1">
         <v>1403</v>
@@ -17413,7 +17410,7 @@
         <v>1440</v>
       </c>
       <c r="B907" s="1" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="908" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -17421,7 +17418,7 @@
         <v>1441</v>
       </c>
       <c r="B908" s="1" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="909" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -17429,7 +17426,7 @@
         <v>1442</v>
       </c>
       <c r="B909" s="1" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="910" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -17454,7 +17451,7 @@
         <v>1444</v>
       </c>
       <c r="B911" s="1" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="912" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -17547,15 +17544,15 @@
         <v>1461</v>
       </c>
       <c r="B917" s="8" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="918" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A918" s="4" t="s">
-        <v>2206</v>
+        <v>2205</v>
       </c>
       <c r="B918" s="8" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="919" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -17563,7 +17560,7 @@
         <v>1456</v>
       </c>
       <c r="B919" s="8" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="920" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -17571,7 +17568,7 @@
         <v>1457</v>
       </c>
       <c r="B920" s="8" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="921" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -17579,7 +17576,7 @@
         <v>1458</v>
       </c>
       <c r="B921" s="8" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="922" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -17587,7 +17584,7 @@
         <v>1459</v>
       </c>
       <c r="B922" s="8" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="923" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -17595,7 +17592,7 @@
         <v>1460</v>
       </c>
       <c r="B923" s="8" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="924" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -17756,7 +17753,7 @@
         <v>1488</v>
       </c>
       <c r="B933" s="1" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="C933" s="1">
         <v>1523</v>
@@ -17773,7 +17770,7 @@
         <v>1489</v>
       </c>
       <c r="B934" s="1" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="C934" s="1">
         <v>479</v>
@@ -17892,7 +17889,7 @@
         <v>1511</v>
       </c>
       <c r="B941" s="10" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="C941" s="1">
         <v>1536</v>
@@ -17926,7 +17923,7 @@
         <v>1514</v>
       </c>
       <c r="B943" s="10" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="C943" s="1">
         <v>1819</v>
@@ -17943,7 +17940,7 @@
         <v>1515</v>
       </c>
       <c r="B944" s="1" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="C944" s="1">
         <v>923</v>
@@ -18223,7 +18220,7 @@
         <v>1558</v>
       </c>
       <c r="B961" s="1" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
       <c r="C961" s="1">
         <v>709</v>
@@ -18240,7 +18237,7 @@
         <v>1559</v>
       </c>
       <c r="B962" s="10" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="C962" s="1">
         <v>2271</v>
@@ -18257,7 +18254,7 @@
         <v>1562</v>
       </c>
       <c r="B963" s="1" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="C963" s="1">
         <v>1917</v>
@@ -18359,7 +18356,7 @@
         <v>1582</v>
       </c>
       <c r="B969" s="10" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="970" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -18367,7 +18364,7 @@
         <v>1583</v>
       </c>
       <c r="B970" s="10" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="971" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -18404,7 +18401,7 @@
     </row>
     <row r="975" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A975" s="4" t="s">
-        <v>2221</v>
+        <v>2220</v>
       </c>
       <c r="B975" s="8" t="s">
         <v>1929</v>
@@ -18486,7 +18483,7 @@
     </row>
     <row r="983" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A983" s="4" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
       <c r="B983" s="1" t="s">
         <v>1955</v>
@@ -18494,7 +18491,7 @@
     </row>
     <row r="984" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A984" s="4" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
       <c r="B984" s="1" t="s">
         <v>1955</v>
@@ -18521,7 +18518,7 @@
         <v>1603</v>
       </c>
       <c r="B987" s="8" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="988" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -18529,7 +18526,7 @@
         <v>1604</v>
       </c>
       <c r="B988" s="8" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="989" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -18537,7 +18534,7 @@
         <v>1605</v>
       </c>
       <c r="B989" s="10" t="s">
-        <v>1956</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="990" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -18550,7 +18547,7 @@
         <v>1607</v>
       </c>
       <c r="B991" s="1" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="992" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -19009,7 +19006,7 @@
         <v>1675</v>
       </c>
       <c r="B1030" s="1" t="s">
-        <v>2139</v>
+        <v>2138</v>
       </c>
       <c r="C1030" s="1">
         <v>1817</v>
@@ -19109,7 +19106,7 @@
         <v>1694</v>
       </c>
       <c r="B1038" s="1" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="1039" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -19554,7 +19551,7 @@
         <v>1766</v>
       </c>
       <c r="B1082" s="1" t="s">
-        <v>2188</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="1083" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -19562,7 +19559,7 @@
         <v>1767</v>
       </c>
       <c r="B1083" s="1" t="s">
-        <v>2188</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="1084" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added doculect Surubonamaram (kt, num)
</commit_message>
<xml_diff>
--- a/raw/concept_mapping.xlsx
+++ b/raw/concept_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bibiko/Documents/Developments/DLCE/lexibank/vanuatuvoices/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0EF82A-C7E7-0147-85B3-9A4F2C459521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C1A4FC-33EE-4242-BDD8-32E909F41D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13040" yWindow="760" windowWidth="21460" windowHeight="17940" xr2:uid="{5A3C358A-0268-8E4B-8A6A-856DEB801F9E}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="vanuatu_all_concepts_6" localSheetId="0">Sheet1!$A$1:$E$1221</definedName>
+    <definedName name="vanuatu_all_concepts_6" localSheetId="0">Sheet1!$A$1:$E$1222</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1028,7 +1028,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3213" uniqueCount="2363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3217" uniqueCount="2364">
   <si>
     <t>org_gloss</t>
   </si>
@@ -8117,6 +8117,9 @@
   </si>
   <si>
     <t>who?</t>
+  </si>
+  <si>
+    <t>yougner_sister</t>
   </si>
 </sst>
 </file>
@@ -8553,11 +8556,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB4F71D-8BFD-5F46-AF6D-0020130BA50C}">
-  <dimension ref="A1:E1258"/>
+  <dimension ref="A1:E1259"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1118" sqref="A1118"/>
+      <pane ySplit="1" topLeftCell="A1169" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1182" sqref="A1182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -21713,57 +21716,66 @@
     </row>
     <row r="1188" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1188" s="4" t="s">
-        <v>1787</v>
+        <v>2363</v>
       </c>
       <c r="B1188" s="1" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="C1188" s="1">
-        <v>1760</v>
+        <v>1761</v>
       </c>
       <c r="D1188" s="6" t="s">
-        <v>1875</v>
+        <v>1873</v>
       </c>
       <c r="E1188" s="6" t="s">
-        <v>1876</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="1189" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1189" s="4" t="s">
-        <v>1788</v>
+        <v>1787</v>
+      </c>
+      <c r="B1189" s="1" t="s">
+        <v>1918</v>
+      </c>
+      <c r="C1189" s="1">
+        <v>1760</v>
+      </c>
+      <c r="D1189" s="6" t="s">
+        <v>1875</v>
+      </c>
+      <c r="E1189" s="6" t="s">
+        <v>1876</v>
       </c>
     </row>
     <row r="1190" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1190" s="4" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="1191" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1191" s="4" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="1192" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1192" s="4" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="1193" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1193" s="4" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="1194" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1194" s="4" t="s">
-        <v>1793</v>
-      </c>
-      <c r="B1194" s="1" t="s">
-        <v>1919</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="1195" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1195" s="4" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="B1195" s="1" t="s">
         <v>1919</v>
@@ -21771,15 +21783,15 @@
     </row>
     <row r="1196" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1196" s="4" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="B1196" s="1" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="1197" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1197" s="4" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="B1197" s="1" t="s">
         <v>1920</v>
@@ -21787,122 +21799,122 @@
     </row>
     <row r="1198" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1198" s="4" t="s">
-        <v>1797</v>
-      </c>
-      <c r="B1198" s="10" t="s">
-        <v>1921</v>
+        <v>1796</v>
+      </c>
+      <c r="B1198" s="1" t="s">
+        <v>1920</v>
       </c>
     </row>
     <row r="1199" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1199" s="4" t="s">
-        <v>1798</v>
-      </c>
-      <c r="B1199" s="1" t="s">
-        <v>1919</v>
+        <v>1797</v>
+      </c>
+      <c r="B1199" s="10" t="s">
+        <v>1921</v>
       </c>
     </row>
     <row r="1200" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1200" s="4" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="B1200" s="1" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="1201" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1201" s="4" t="s">
-        <v>1800</v>
+        <v>1799</v>
+      </c>
+      <c r="B1201" s="1" t="s">
+        <v>1920</v>
       </c>
     </row>
     <row r="1202" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1202" s="4" t="s">
-        <v>1801</v>
-      </c>
-      <c r="B1202" s="1" t="s">
-        <v>1915</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="1203" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1203" s="4" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="B1203" s="1" t="s">
-        <v>1914</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="1204" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1204" s="4" t="s">
-        <v>1803</v>
+        <v>1802</v>
+      </c>
+      <c r="B1204" s="1" t="s">
+        <v>1914</v>
       </c>
     </row>
     <row r="1205" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1205" s="4" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="1206" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1206" s="4" t="s">
-        <v>1805</v>
-      </c>
-      <c r="B1206" s="1" t="s">
-        <v>1917</v>
-      </c>
-      <c r="C1206" s="1">
-        <v>1761</v>
-      </c>
-      <c r="D1206" s="6" t="s">
-        <v>1873</v>
-      </c>
-      <c r="E1206" s="6" t="s">
-        <v>1874</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="1207" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1207" s="4" t="s">
-        <v>1806</v>
+        <v>1805</v>
+      </c>
+      <c r="B1207" s="1" t="s">
+        <v>1917</v>
+      </c>
+      <c r="C1207" s="1">
+        <v>1761</v>
+      </c>
+      <c r="D1207" s="6" t="s">
+        <v>1873</v>
+      </c>
+      <c r="E1207" s="6" t="s">
+        <v>1874</v>
       </c>
     </row>
     <row r="1208" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1208" s="4" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="1209" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1209" s="4" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="1210" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1210" s="4" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="1211" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1211" s="4" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
     </row>
     <row r="1212" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1212" s="4" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="1213" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1213" s="4" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="1214" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1214" s="4" t="s">
-        <v>1813</v>
-      </c>
-      <c r="B1214" s="1" t="s">
-        <v>1922</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="1215" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1215" s="4" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="B1215" s="1" t="s">
         <v>1922</v>
@@ -21910,15 +21922,15 @@
     </row>
     <row r="1216" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1216" s="4" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="B1216" s="1" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="1217" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1217" s="4" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="B1217" s="1" t="s">
         <v>1923</v>
@@ -21926,347 +21938,344 @@
     </row>
     <row r="1218" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1218" s="4" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="B1218" s="1" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="1219" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1219" s="4" t="s">
-        <v>1818</v>
-      </c>
-      <c r="B1219" s="10" t="s">
-        <v>1925</v>
+        <v>1817</v>
+      </c>
+      <c r="B1219" s="1" t="s">
+        <v>1924</v>
       </c>
     </row>
     <row r="1220" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1220" s="4" t="s">
-        <v>1819</v>
-      </c>
-      <c r="B1220" s="1" t="s">
-        <v>1922</v>
+        <v>1818</v>
+      </c>
+      <c r="B1220" s="10" t="s">
+        <v>1925</v>
       </c>
     </row>
     <row r="1221" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1221" s="4" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="B1221" s="1" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="1222" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1222" s="4" t="s">
-        <v>2243</v>
+        <v>1820</v>
       </c>
       <c r="B1222" s="1" t="s">
-        <v>2244</v>
-      </c>
-      <c r="C1222" s="1">
-        <v>1256</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="1223" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1223" s="4" t="s">
-        <v>2250</v>
+        <v>2243</v>
       </c>
       <c r="B1223" s="1" t="s">
-        <v>2251</v>
+        <v>2244</v>
       </c>
       <c r="C1223" s="1">
-        <v>1416</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="1224" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1224" s="4" t="s">
-        <v>2254</v>
+        <v>2250</v>
       </c>
       <c r="B1224" s="1" t="s">
-        <v>2255</v>
+        <v>2251</v>
       </c>
       <c r="C1224" s="1">
-        <v>2105</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="1225" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1225" s="4" t="s">
-        <v>2256</v>
+        <v>2254</v>
       </c>
       <c r="B1225" s="1" t="s">
-        <v>2236</v>
+        <v>2255</v>
       </c>
       <c r="C1225" s="1">
-        <v>1094</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="1226" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1226" s="4" t="s">
-        <v>2260</v>
+        <v>2256</v>
       </c>
       <c r="B1226" s="1" t="s">
-        <v>2261</v>
+        <v>2236</v>
       </c>
       <c r="C1226" s="1">
-        <v>1433</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="1227" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1227" s="4" t="s">
-        <v>2275</v>
+        <v>2260</v>
       </c>
       <c r="B1227" s="1" t="s">
-        <v>2276</v>
+        <v>2261</v>
       </c>
       <c r="C1227" s="1">
-        <v>1156</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="1228" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1228" s="4" t="s">
-        <v>2278</v>
+        <v>2275</v>
       </c>
       <c r="B1228" s="1" t="s">
-        <v>2279</v>
+        <v>2276</v>
       </c>
       <c r="C1228" s="1">
-        <v>1456</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="1229" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1229" s="4" t="s">
-        <v>2280</v>
+        <v>2278</v>
       </c>
       <c r="B1229" s="1" t="s">
-        <v>2281</v>
+        <v>2279</v>
       </c>
       <c r="C1229" s="1">
-        <v>1280</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="1230" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1230" s="4" t="s">
-        <v>2282</v>
+        <v>2280</v>
       </c>
       <c r="B1230" s="1" t="s">
-        <v>2283</v>
+        <v>2281</v>
       </c>
       <c r="C1230" s="1">
-        <v>2009</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="1231" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1231" s="4" t="s">
-        <v>2284</v>
+        <v>2282</v>
       </c>
       <c r="B1231" s="1" t="s">
-        <v>2285</v>
+        <v>2283</v>
       </c>
       <c r="C1231" s="1">
-        <v>937</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1232" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1232" s="4" t="s">
-        <v>2286</v>
+        <v>2284</v>
       </c>
       <c r="B1232" s="1" t="s">
-        <v>2287</v>
+        <v>2285</v>
       </c>
       <c r="C1232" s="1">
-        <v>744</v>
+        <v>937</v>
       </c>
     </row>
     <row r="1233" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1233" s="4" t="s">
-        <v>2288</v>
+        <v>2286</v>
       </c>
       <c r="B1233" s="1" t="s">
-        <v>2289</v>
+        <v>2287</v>
       </c>
       <c r="C1233" s="1">
-        <v>1201</v>
+        <v>744</v>
       </c>
     </row>
     <row r="1234" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1234" s="4" t="s">
-        <v>2290</v>
+        <v>2288</v>
       </c>
       <c r="B1234" s="1" t="s">
-        <v>1826</v>
+        <v>2289</v>
       </c>
       <c r="C1234" s="1">
-        <v>1441</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="1235" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1235" s="4" t="s">
-        <v>2291</v>
+        <v>2290</v>
       </c>
       <c r="B1235" s="1" t="s">
-        <v>2292</v>
+        <v>1826</v>
       </c>
       <c r="C1235" s="1">
-        <v>1282</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="1236" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1236" s="4" t="s">
-        <v>2293</v>
+        <v>2291</v>
       </c>
       <c r="B1236" s="1" t="s">
-        <v>2294</v>
+        <v>2292</v>
       </c>
       <c r="C1236" s="1">
-        <v>1220</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="1237" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1237" s="4" t="s">
-        <v>2296</v>
+        <v>2293</v>
       </c>
       <c r="B1237" s="1" t="s">
-        <v>2295</v>
+        <v>2294</v>
       </c>
       <c r="C1237" s="1">
-        <v>1392</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="1238" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1238" s="4" t="s">
-        <v>2297</v>
+        <v>2296</v>
       </c>
       <c r="B1238" s="1" t="s">
-        <v>2151</v>
+        <v>2295</v>
       </c>
       <c r="C1238" s="1">
-        <v>670</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="1239" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1239" s="4" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
       <c r="B1239" s="1" t="s">
-        <v>1827</v>
+        <v>2151</v>
       </c>
       <c r="C1239" s="1">
-        <v>1228</v>
+        <v>670</v>
       </c>
     </row>
     <row r="1240" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1240" s="4" t="s">
-        <v>2300</v>
+        <v>2298</v>
       </c>
       <c r="B1240" s="1" t="s">
-        <v>2299</v>
+        <v>1827</v>
       </c>
       <c r="C1240" s="1">
-        <v>671</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="1241" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1241" s="4" t="s">
-        <v>2301</v>
+        <v>2300</v>
       </c>
       <c r="B1241" s="1" t="s">
-        <v>2234</v>
+        <v>2299</v>
       </c>
       <c r="C1241" s="1">
-        <v>420</v>
+        <v>671</v>
       </c>
     </row>
     <row r="1242" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1242" s="4" t="s">
-        <v>2303</v>
+        <v>2301</v>
       </c>
       <c r="B1242" s="1" t="s">
-        <v>2302</v>
+        <v>2234</v>
       </c>
       <c r="C1242" s="1">
-        <v>249</v>
+        <v>420</v>
       </c>
     </row>
     <row r="1243" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1243" s="4" t="s">
-        <v>2305</v>
+        <v>2303</v>
       </c>
       <c r="B1243" s="1" t="s">
-        <v>2304</v>
+        <v>2302</v>
       </c>
       <c r="C1243" s="1">
-        <v>2103</v>
+        <v>249</v>
       </c>
     </row>
     <row r="1244" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1244" s="4" t="s">
-        <v>2306</v>
+        <v>2305</v>
       </c>
       <c r="B1244" s="1" t="s">
-        <v>1822</v>
+        <v>2304</v>
       </c>
       <c r="C1244" s="1">
-        <v>487</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="1245" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1245" s="4" t="s">
-        <v>2307</v>
+        <v>2306</v>
       </c>
       <c r="B1245" s="1" t="s">
-        <v>1831</v>
+        <v>1822</v>
       </c>
       <c r="C1245" s="1">
-        <v>1460</v>
+        <v>487</v>
       </c>
     </row>
     <row r="1246" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1246" s="4" t="s">
-        <v>2308</v>
+        <v>2307</v>
       </c>
       <c r="B1246" s="1" t="s">
-        <v>1834</v>
+        <v>1831</v>
       </c>
       <c r="C1246" s="1">
-        <v>1741</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="1247" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1247" s="4" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="B1247" s="1" t="s">
-        <v>1824</v>
+        <v>1834</v>
       </c>
       <c r="C1247" s="1">
-        <v>1485</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="1248" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1248" s="4" t="s">
-        <v>615</v>
+        <v>2309</v>
       </c>
       <c r="B1248" s="1" t="s">
-        <v>1830</v>
+        <v>1824</v>
       </c>
       <c r="C1248" s="1">
-        <v>1209</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="1249" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1249" s="4" t="s">
-        <v>2310</v>
+        <v>615</v>
       </c>
       <c r="B1249" s="1" t="s">
-        <v>1829</v>
+        <v>1830</v>
       </c>
       <c r="C1249" s="1">
-        <v>2642</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="1250" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1250" s="4" t="s">
-        <v>2352</v>
+        <v>2310</v>
       </c>
       <c r="B1250" s="1" t="s">
         <v>1829</v>
@@ -22277,18 +22286,18 @@
     </row>
     <row r="1251" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1251" s="4" t="s">
-        <v>2311</v>
+        <v>2352</v>
       </c>
       <c r="B1251" s="1" t="s">
-        <v>1837</v>
+        <v>1829</v>
       </c>
       <c r="C1251" s="1">
-        <v>1131</v>
+        <v>2642</v>
       </c>
     </row>
     <row r="1252" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1252" s="4" t="s">
-        <v>2357</v>
+        <v>2311</v>
       </c>
       <c r="B1252" s="1" t="s">
         <v>1837</v>
@@ -22299,18 +22308,18 @@
     </row>
     <row r="1253" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1253" s="4" t="s">
-        <v>2312</v>
+        <v>2357</v>
       </c>
       <c r="B1253" s="1" t="s">
-        <v>1839</v>
+        <v>1837</v>
       </c>
       <c r="C1253" s="1">
-        <v>1130</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="1254" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1254" s="4" t="s">
-        <v>2358</v>
+        <v>2312</v>
       </c>
       <c r="B1254" s="1" t="s">
         <v>1839</v>
@@ -22321,29 +22330,29 @@
     </row>
     <row r="1255" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1255" s="4" t="s">
-        <v>2313</v>
+        <v>2358</v>
       </c>
       <c r="B1255" s="1" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="C1255" s="1">
-        <v>2637</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="1256" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1256" s="4" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
       <c r="B1256" s="1" t="s">
-        <v>1838</v>
+        <v>1840</v>
       </c>
       <c r="C1256" s="1">
-        <v>2636</v>
+        <v>2637</v>
       </c>
     </row>
     <row r="1257" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1257" s="4" t="s">
-        <v>2353</v>
+        <v>2314</v>
       </c>
       <c r="B1257" s="1" t="s">
         <v>1838</v>
@@ -22354,12 +22363,23 @@
     </row>
     <row r="1258" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1258" s="4" t="s">
+        <v>2353</v>
+      </c>
+      <c r="B1258" s="1" t="s">
+        <v>1838</v>
+      </c>
+      <c r="C1258" s="1">
+        <v>2636</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1259" s="4" t="s">
         <v>2335</v>
       </c>
-      <c r="B1258" s="1" t="s">
+      <c r="B1259" s="1" t="s">
         <v>2281</v>
       </c>
-      <c r="C1258" s="1">
+      <c r="C1259" s="1">
         <v>1280</v>
       </c>
     </row>

</xml_diff>